<commit_message>
update run_settings tab in thoipapy_standalone_run_settings.xlsx, which only affects tests against protein sets, not standalone predictions
</commit_message>
<xml_diff>
--- a/thoipapy/setting/thoipapy_standalone_run_settings.xlsx
+++ b/thoipapy/setting/thoipapy_standalone_run_settings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="run_settings" sheetId="1" state="visible" r:id="rId2"/>
@@ -1107,7 +1107,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1273,14 +1273,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1392,11 +1384,11 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.43"/>
@@ -1406,7 +1398,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1423,12 +1415,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>
@@ -1440,7 +1432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1455,7 +1447,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
@@ -1470,7 +1462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
@@ -1483,7 +1475,7 @@
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -1500,7 +1492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
         <v>17</v>
       </c>
@@ -1515,7 +1507,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
@@ -1574,7 +1566,7 @@
         <v>28</v>
       </c>
       <c r="B12" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>29</v>
@@ -1591,7 +1583,7 @@
         <v>30</v>
       </c>
       <c r="B13" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13" t="s">
@@ -1606,7 +1598,7 @@
         <v>31</v>
       </c>
       <c r="B14" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>32</v>
@@ -1623,7 +1615,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>35</v>
@@ -1640,7 +1632,7 @@
         <v>36</v>
       </c>
       <c r="B16" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>37</v>
@@ -1653,7 +1645,7 @@
         <v>38</v>
       </c>
       <c r="B17" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>39</v>
@@ -1670,7 +1662,7 @@
         <v>40</v>
       </c>
       <c r="B18" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>41</v>
@@ -1687,7 +1679,7 @@
         <v>42</v>
       </c>
       <c r="B19" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>43</v>
@@ -1704,7 +1696,7 @@
         <v>44</v>
       </c>
       <c r="B20" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>45</v>
@@ -1721,7 +1713,7 @@
         <v>46</v>
       </c>
       <c r="B21" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="16" t="s">
@@ -1736,7 +1728,7 @@
         <v>47</v>
       </c>
       <c r="B22" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>48</v>
@@ -1753,7 +1745,7 @@
         <v>49</v>
       </c>
       <c r="B23" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>50</v>
@@ -1832,7 +1824,7 @@
         <v>58</v>
       </c>
       <c r="B28" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="22" t="s">
         <v>59</v>
@@ -1889,7 +1881,7 @@
       <c r="D31" s="27"/>
       <c r="E31" s="28"/>
     </row>
-    <row r="32" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="29" t="s">
         <v>65</v>
       </c>
@@ -1904,7 +1896,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="27" t="s">
         <v>67</v>
       </c>
@@ -1915,12 +1907,12 @@
       <c r="D33" s="27"/>
       <c r="E33" s="28"/>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="30" t="s">
         <v>68</v>
       </c>
       <c r="B34" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="30"/>
       <c r="D34" s="31" t="s">
@@ -1930,7 +1922,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="30" t="s">
         <v>70</v>
       </c>
@@ -1947,7 +1939,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="31" t="s">
         <v>72</v>
       </c>
@@ -1964,7 +1956,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="31" t="s">
         <v>76</v>
       </c>
@@ -1979,7 +1971,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="31" t="s">
         <v>78</v>
       </c>
@@ -1994,7 +1986,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
         <v>79</v>
       </c>
@@ -2011,7 +2003,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
         <v>82</v>
       </c>
@@ -2124,7 +2116,7 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -2348,10 +2340,10 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="B23" s="43" t="n">
+      <c r="B23" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C23" s="0" t="s">
@@ -2521,7 +2513,7 @@
       <c r="A40" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="42" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2529,7 +2521,7 @@
       <c r="A41" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B41" s="45" t="s">
+      <c r="B41" s="43" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2541,10 +2533,10 @@
       <c r="C42" s="40"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="B43" s="44" t="n">
+      <c r="B43" s="42" t="n">
         <v>0.35</v>
       </c>
     </row>
@@ -2552,7 +2544,7 @@
       <c r="A44" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B44" s="44" t="n">
+      <c r="B44" s="42" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2560,7 +2552,7 @@
       <c r="A45" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B45" s="44" t="n">
+      <c r="B45" s="42" t="n">
         <v>0.2</v>
       </c>
     </row>
@@ -2568,7 +2560,7 @@
       <c r="A46" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B46" s="44" t="n">
+      <c r="B46" s="42" t="n">
         <v>6</v>
       </c>
     </row>
@@ -2576,7 +2568,7 @@
       <c r="A47" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="B47" s="44" t="n">
+      <c r="B47" s="42" t="n">
         <v>0.8</v>
       </c>
     </row>
@@ -2699,10 +2691,10 @@
       <c r="A1" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="45" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2710,10 +2702,10 @@
       <c r="A2" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="49" t="s">
+      <c r="B2" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="47" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2721,10 +2713,10 @@
       <c r="A3" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="47" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2732,10 +2724,10 @@
       <c r="A4" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="49" t="s">
+      <c r="B4" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="47" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2743,10 +2735,10 @@
       <c r="A5" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="B5" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="49" t="s">
+      <c r="B5" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="47" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2754,10 +2746,10 @@
       <c r="A6" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="B6" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="49" t="s">
+      <c r="B6" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="47" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2765,10 +2757,10 @@
       <c r="A7" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="B7" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="49" t="s">
+      <c r="B7" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="47" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2779,7 +2771,7 @@
       <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="47" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2790,7 +2782,7 @@
       <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="47" t="s">
         <v>175</v>
       </c>
     </row>
@@ -2801,7 +2793,7 @@
       <c r="B10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2812,7 +2804,7 @@
       <c r="B11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2823,7 +2815,7 @@
       <c r="B12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2834,7 +2826,7 @@
       <c r="B13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2845,7 +2837,7 @@
       <c r="B14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2856,7 +2848,7 @@
       <c r="B15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2867,7 +2859,7 @@
       <c r="B16" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2878,7 +2870,7 @@
       <c r="B17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2889,7 +2881,7 @@
       <c r="B18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2900,7 +2892,7 @@
       <c r="B19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2911,7 +2903,7 @@
       <c r="B20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2922,7 +2914,7 @@
       <c r="B21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C21" s="49" t="s">
+      <c r="C21" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2933,7 +2925,7 @@
       <c r="B22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2944,7 +2936,7 @@
       <c r="B23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2955,7 +2947,7 @@
       <c r="B24" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2966,7 +2958,7 @@
       <c r="B25" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2977,7 +2969,7 @@
       <c r="B26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="C26" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2988,7 +2980,7 @@
       <c r="B27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2999,7 +2991,7 @@
       <c r="B28" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C28" s="50" t="s">
+      <c r="C28" s="48" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3010,7 +3002,7 @@
       <c r="B29" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3021,7 +3013,7 @@
       <c r="B30" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C30" s="49" t="s">
+      <c r="C30" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3032,7 +3024,7 @@
       <c r="B31" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C31" s="49" t="s">
+      <c r="C31" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3043,7 +3035,7 @@
       <c r="B32" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C32" s="49" t="s">
+      <c r="C32" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3054,7 +3046,7 @@
       <c r="B33" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3065,7 +3057,7 @@
       <c r="B34" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C34" s="49" t="s">
+      <c r="C34" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3076,7 +3068,7 @@
       <c r="B35" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3087,7 +3079,7 @@
       <c r="B36" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C36" s="49" t="s">
+      <c r="C36" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3098,7 +3090,7 @@
       <c r="B37" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C37" s="49" t="s">
+      <c r="C37" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3109,7 +3101,7 @@
       <c r="B38" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3120,7 +3112,7 @@
       <c r="B39" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C39" s="49" t="s">
+      <c r="C39" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3131,7 +3123,7 @@
       <c r="B40" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C40" s="49" t="s">
+      <c r="C40" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3142,7 +3134,7 @@
       <c r="B41" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C41" s="49" t="s">
+      <c r="C41" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3153,7 +3145,7 @@
       <c r="B42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3164,7 +3156,7 @@
       <c r="B43" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C43" s="49" t="s">
+      <c r="C43" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3175,7 +3167,7 @@
       <c r="B44" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C44" s="49" t="s">
+      <c r="C44" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3186,7 +3178,7 @@
       <c r="B45" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C45" s="49" t="s">
+      <c r="C45" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3194,10 +3186,10 @@
       <c r="A46" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="B46" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C46" s="49" t="s">
+      <c r="B46" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3205,10 +3197,10 @@
       <c r="A47" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="B47" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C47" s="49" t="s">
+      <c r="B47" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3216,10 +3208,10 @@
       <c r="A48" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="B48" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C48" s="49" t="s">
+      <c r="B48" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" s="47" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3227,10 +3219,10 @@
       <c r="A49" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="B49" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C49" s="49" t="s">
+      <c r="B49" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3238,10 +3230,10 @@
       <c r="A50" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B50" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C50" s="49" t="s">
+      <c r="B50" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" s="47" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3252,7 +3244,7 @@
       <c r="B51" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C51" s="49" t="s">
+      <c r="C51" s="47" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3263,7 +3255,7 @@
       <c r="B52" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C52" s="49" t="s">
+      <c r="C52" s="47" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3274,7 +3266,7 @@
       <c r="B53" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C53" s="49" t="s">
+      <c r="C53" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3285,7 +3277,7 @@
       <c r="B54" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C54" s="49" t="s">
+      <c r="C54" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3296,7 +3288,7 @@
       <c r="B55" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C55" s="49" t="s">
+      <c r="C55" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3307,7 +3299,7 @@
       <c r="B56" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C56" s="49" t="s">
+      <c r="C56" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3318,7 +3310,7 @@
       <c r="B57" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C57" s="49" t="s">
+      <c r="C57" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3329,7 +3321,7 @@
       <c r="B58" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C58" s="49" t="s">
+      <c r="C58" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3340,7 +3332,7 @@
       <c r="B59" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C59" s="49" t="s">
+      <c r="C59" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3351,7 +3343,7 @@
       <c r="B60" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C60" s="49" t="s">
+      <c r="C60" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3362,7 +3354,7 @@
       <c r="B61" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C61" s="49" t="s">
+      <c r="C61" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3373,7 +3365,7 @@
       <c r="B62" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C62" s="49" t="s">
+      <c r="C62" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3384,7 +3376,7 @@
       <c r="B63" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C63" s="49" t="s">
+      <c r="C63" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3395,7 +3387,7 @@
       <c r="B64" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C64" s="49" t="s">
+      <c r="C64" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3406,7 +3398,7 @@
       <c r="B65" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C65" s="49" t="s">
+      <c r="C65" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3417,7 +3409,7 @@
       <c r="B66" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C66" s="49" t="s">
+      <c r="C66" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3428,7 +3420,7 @@
       <c r="B67" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C67" s="49" t="s">
+      <c r="C67" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3439,7 +3431,7 @@
       <c r="B68" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C68" s="49" t="s">
+      <c r="C68" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3450,7 +3442,7 @@
       <c r="B69" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C69" s="49" t="s">
+      <c r="C69" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3461,7 +3453,7 @@
       <c r="B70" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C70" s="49" t="s">
+      <c r="C70" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3472,7 +3464,7 @@
       <c r="B71" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C71" s="49" t="s">
+      <c r="C71" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3483,7 +3475,7 @@
       <c r="B72" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C72" s="49" t="s">
+      <c r="C72" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3494,7 +3486,7 @@
       <c r="B73" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C73" s="49" t="s">
+      <c r="C73" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3505,7 +3497,7 @@
       <c r="B74" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C74" s="49" t="s">
+      <c r="C74" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3516,7 +3508,7 @@
       <c r="B75" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C75" s="49" t="s">
+      <c r="C75" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3527,7 +3519,7 @@
       <c r="B76" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C76" s="49" t="s">
+      <c r="C76" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3538,7 +3530,7 @@
       <c r="B77" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C77" s="49" t="s">
+      <c r="C77" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3549,7 +3541,7 @@
       <c r="B78" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C78" s="49" t="s">
+      <c r="C78" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3560,7 +3552,7 @@
       <c r="B79" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C79" s="49" t="s">
+      <c r="C79" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3571,7 +3563,7 @@
       <c r="B80" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C80" s="49" t="s">
+      <c r="C80" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3582,7 +3574,7 @@
       <c r="B81" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C81" s="49" t="s">
+      <c r="C81" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3593,7 +3585,7 @@
       <c r="B82" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C82" s="49" t="s">
+      <c r="C82" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3604,7 +3596,7 @@
       <c r="B83" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C83" s="49" t="s">
+      <c r="C83" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3615,7 +3607,7 @@
       <c r="B84" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C84" s="49" t="s">
+      <c r="C84" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3626,7 +3618,7 @@
       <c r="B85" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C85" s="49" t="s">
+      <c r="C85" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3637,7 +3629,7 @@
       <c r="B86" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C86" s="49" t="s">
+      <c r="C86" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3648,7 +3640,7 @@
       <c r="B87" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C87" s="49" t="s">
+      <c r="C87" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3659,7 +3651,7 @@
       <c r="B88" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C88" s="49" t="s">
+      <c r="C88" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3670,7 +3662,7 @@
       <c r="B89" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C89" s="49" t="s">
+      <c r="C89" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3681,7 +3673,7 @@
       <c r="B90" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C90" s="49" t="s">
+      <c r="C90" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3692,7 +3684,7 @@
       <c r="B91" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C91" s="49" t="s">
+      <c r="C91" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3703,7 +3695,7 @@
       <c r="B92" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C92" s="49" t="s">
+      <c r="C92" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3714,7 +3706,7 @@
       <c r="B93" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C93" s="49" t="s">
+      <c r="C93" s="47" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3725,7 +3717,7 @@
       <c r="B94" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C94" s="49" t="s">
+      <c r="C94" s="47" t="s">
         <v>264</v>
       </c>
     </row>
@@ -3736,7 +3728,7 @@
       <c r="B95" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C95" s="49" t="s">
+      <c r="C95" s="47" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3747,7 +3739,7 @@
       <c r="B96" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C96" s="49" t="s">
+      <c r="C96" s="47" t="s">
         <v>264</v>
       </c>
     </row>
@@ -3758,7 +3750,7 @@
       <c r="B97" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C97" s="49" t="s">
+      <c r="C97" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3766,10 +3758,10 @@
       <c r="A98" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="B98" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C98" s="49" t="s">
+      <c r="B98" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C98" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3780,7 +3772,7 @@
       <c r="B99" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C99" s="49" t="s">
+      <c r="C99" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3791,7 +3783,7 @@
       <c r="B100" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C100" s="49" t="s">
+      <c r="C100" s="47" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3802,7 +3794,7 @@
       <c r="B101" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C101" s="49" t="s">
+      <c r="C101" s="47" t="s">
         <v>272</v>
       </c>
     </row>
@@ -3813,7 +3805,7 @@
       <c r="B102" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C102" s="49" t="s">
+      <c r="C102" s="47" t="s">
         <v>272</v>
       </c>
     </row>
@@ -3824,7 +3816,7 @@
       <c r="B103" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C103" s="49" t="s">
+      <c r="C103" s="47" t="s">
         <v>272</v>
       </c>
     </row>
@@ -3835,7 +3827,7 @@
       <c r="B104" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C104" s="49" t="s">
+      <c r="C104" s="47" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3843,10 +3835,10 @@
       <c r="A105" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="B105" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C105" s="49" t="s">
+      <c r="B105" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C105" s="47" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3857,7 +3849,7 @@
       <c r="B106" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C106" s="49" t="s">
+      <c r="C106" s="47" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3868,7 +3860,7 @@
       <c r="B107" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C107" s="49" t="s">
+      <c r="C107" s="47" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3879,7 +3871,7 @@
       <c r="B108" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C108" s="49" t="s">
+      <c r="C108" s="47" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3890,7 +3882,7 @@
       <c r="B109" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C109" s="49" t="s">
+      <c r="C109" s="47" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3901,7 +3893,7 @@
       <c r="B110" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C110" s="49" t="s">
+      <c r="C110" s="47" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3912,7 +3904,7 @@
       <c r="B111" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C111" s="49" t="s">
+      <c r="C111" s="47" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3923,7 +3915,7 @@
       <c r="B112" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C112" s="49" t="s">
+      <c r="C112" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3934,7 +3926,7 @@
       <c r="B113" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C113" s="49" t="s">
+      <c r="C113" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3945,7 +3937,7 @@
       <c r="B114" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C114" s="49" t="s">
+      <c r="C114" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3956,7 +3948,7 @@
       <c r="B115" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C115" s="49" t="s">
+      <c r="C115" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3967,7 +3959,7 @@
       <c r="B116" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C116" s="49" t="s">
+      <c r="C116" s="47" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3978,7 +3970,7 @@
       <c r="B117" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C117" s="49" t="s">
+      <c r="C117" s="47" t="s">
         <v>177</v>
       </c>
     </row>

</xml_diff>